<commit_message>
[IMP] Temporary save 20220401
</commit_message>
<xml_diff>
--- a/z0bug_odoo/z0bug_odoo/data/date_range.xlsx
+++ b/z0bug_odoo/z0bug_odoo/data/date_range.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="197">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -509,6 +509,108 @@
   </si>
   <si>
     <t xml:space="preserve">2022/T4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/T1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/T3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.2023-Q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/T4</t>
   </si>
 </sst>
 </file>
@@ -591,16 +693,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -617,1271 +723,1679 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="n">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="n">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="n">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="n">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="n">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="n">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="n">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="n">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1" t="n">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1" t="n">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1" t="n">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1" t="n">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1" t="n">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1" t="n">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1" t="n">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1" t="n">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1" t="n">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1" t="n">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1" t="n">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1" t="n">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="1" t="n">
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="1" t="n">
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1" t="n">
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1" t="n">
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1" t="n">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D37" s="2" t="n">
+      <c r="D37" s="3" t="n">
         <v>44562</v>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E37" s="3" t="n">
         <v>44592</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="1" t="n">
+      <c r="F37" s="2"/>
+      <c r="G37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D38" s="3" t="n">
         <v>44593</v>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E38" s="3" t="n">
         <v>44620</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1" t="n">
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="2" t="n">
+      <c r="D39" s="3" t="n">
         <v>44621</v>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E39" s="3" t="n">
         <v>44651</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1" t="n">
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="D40" s="3" t="n">
         <v>44652</v>
       </c>
-      <c r="E40" s="2" t="n">
+      <c r="E40" s="3" t="n">
         <v>44681</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="1" t="n">
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D41" s="2" t="n">
+      <c r="D41" s="3" t="n">
         <v>44682</v>
       </c>
-      <c r="E41" s="2" t="n">
+      <c r="E41" s="3" t="n">
         <v>44712</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1" t="n">
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="3" t="n">
         <v>44713</v>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="3" t="n">
         <v>44742</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1" t="n">
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="3" t="n">
         <v>44743</v>
       </c>
-      <c r="E43" s="2" t="n">
+      <c r="E43" s="3" t="n">
         <v>44773</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" s="1" t="n">
+      <c r="F43" s="2"/>
+      <c r="G43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="3" t="n">
         <v>44774</v>
       </c>
-      <c r="E44" s="2" t="n">
+      <c r="E44" s="3" t="n">
         <v>44804</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="1" t="n">
+      <c r="F44" s="2"/>
+      <c r="G44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="3" t="n">
         <v>44805</v>
       </c>
-      <c r="E45" s="2" t="n">
+      <c r="E45" s="3" t="n">
         <v>44834</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="1" t="n">
+      <c r="F45" s="2"/>
+      <c r="G45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D46" s="2" t="n">
+      <c r="D46" s="3" t="n">
         <v>44835</v>
       </c>
-      <c r="E46" s="2" t="n">
+      <c r="E46" s="3" t="n">
         <v>44865</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" s="1" t="n">
+      <c r="F46" s="2"/>
+      <c r="G46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="B47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D47" s="2" t="n">
+      <c r="D47" s="3" t="n">
         <v>44866</v>
       </c>
-      <c r="E47" s="2" t="n">
+      <c r="E47" s="3" t="n">
         <v>44895</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H47" s="1" t="n">
+      <c r="F47" s="2"/>
+      <c r="G47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D48" s="2" t="n">
+      <c r="D48" s="3" t="n">
         <v>44896</v>
       </c>
-      <c r="E48" s="2" t="n">
+      <c r="E48" s="3" t="n">
         <v>44926</v>
       </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1" t="n">
+      <c r="F48" s="2"/>
+      <c r="G48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D49" s="2" t="n">
+      <c r="D49" s="3" t="n">
         <v>44562</v>
       </c>
-      <c r="E49" s="2" t="n">
+      <c r="E49" s="3" t="n">
         <v>44651</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H49" s="1" t="n">
+      <c r="F49" s="2"/>
+      <c r="G49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D50" s="2" t="n">
+      <c r="D50" s="3" t="n">
         <v>44652</v>
       </c>
-      <c r="E50" s="2" t="n">
+      <c r="E50" s="3" t="n">
         <v>44742</v>
       </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H50" s="1" t="n">
+      <c r="F50" s="2"/>
+      <c r="G50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D51" s="2" t="n">
+      <c r="D51" s="3" t="n">
         <v>44743</v>
       </c>
-      <c r="E51" s="2" t="n">
+      <c r="E51" s="3" t="n">
         <v>44834</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H51" s="1" t="n">
+      <c r="F51" s="2"/>
+      <c r="G51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D52" s="2" t="n">
+      <c r="D52" s="3" t="n">
         <v>44835</v>
       </c>
-      <c r="E52" s="2" t="n">
+      <c r="E52" s="3" t="n">
         <v>44926</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H52" s="1" t="n">
+      <c r="F52" s="2"/>
+      <c r="G52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>44927</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>45291</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>44927</v>
+      </c>
+      <c r="E54" s="3" t="n">
+        <v>44957</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>44958</v>
+      </c>
+      <c r="E55" s="3" t="n">
+        <v>44985</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>44986</v>
+      </c>
+      <c r="E56" s="3" t="n">
+        <v>45016</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>45017</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>45046</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>45047</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>45077</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>45078</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>45107</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>45108</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>45138</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>45139</v>
+      </c>
+      <c r="E61" s="3" t="n">
+        <v>45169</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>45170</v>
+      </c>
+      <c r="E62" s="3" t="n">
+        <v>45199</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D63" s="3" t="n">
+        <v>45200</v>
+      </c>
+      <c r="E63" s="3" t="n">
+        <v>45230</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" s="3" t="n">
+        <v>45231</v>
+      </c>
+      <c r="E64" s="3" t="n">
+        <v>45260</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D65" s="3" t="n">
+        <v>45261</v>
+      </c>
+      <c r="E65" s="3" t="n">
+        <v>45291</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>44927</v>
+      </c>
+      <c r="E66" s="3" t="n">
+        <v>45016</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>45017</v>
+      </c>
+      <c r="E67" s="3" t="n">
+        <v>45107</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>45108</v>
+      </c>
+      <c r="E68" s="3" t="n">
+        <v>45199</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>45200</v>
+      </c>
+      <c r="E69" s="3" t="n">
+        <v>45291</v>
+      </c>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1891,8 +2405,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>